<commit_message>
Add edited alloy input file template
</commit_message>
<xml_diff>
--- a/Alloy Template.xlsx
+++ b/Alloy Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bama365-my.sharepoint.com/personal/amjordan7_crimson_ua_edu/Documents/Documents/1 Projects/Research/3_AM Alloy Hot Cracking Prediction Project/3_hcsi_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bama365-my.sharepoint.com/personal/amjordan7_crimson_ua_edu/Documents/Documents/1 Projects/Research/3_AM-Hot Cracking ML-CALPHAD Project/3_hcm_calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="525" documentId="8_{21EBF174-53D2-406F-9F3E-90F98D5EF992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C7A319-EAC2-4683-925D-903CE321B0FB}"/>
+  <xr:revisionPtr revIDLastSave="532" documentId="8_{21EBF174-53D2-406F-9F3E-90F98D5EF992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4627661-9CC2-44B9-9C89-6E733B5A3DB9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-10740" windowWidth="16440" windowHeight="29040" tabRatio="497" xr2:uid="{39467DA1-796B-4162-A05F-681B8E420767}"/>
+    <workbookView xWindow="29580" yWindow="-9840" windowWidth="13350" windowHeight="21285" tabRatio="497" xr2:uid="{39467DA1-796B-4162-A05F-681B8E420767}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>Particle Additions</t>
   </si>
@@ -201,6 +201,36 @@
   </si>
   <si>
     <t>Scanning Velo (mm/s)</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1359645421000781</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Al-0.5Si</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>LPBF</t>
+  </si>
+  <si>
+    <t>Al-1.0Si</t>
+  </si>
+  <si>
+    <t>Al-2.0Si</t>
+  </si>
+  <si>
+    <t>Al-4.0Si</t>
+  </si>
+  <si>
+    <t>Al-12.6Si</t>
+  </si>
+  <si>
+    <t>Al-16.0Si</t>
   </si>
 </sst>
 </file>
@@ -613,7 +643,7 @@
   <dimension ref="A1:BB171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,308 +837,941 @@
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1">
+        <v>99.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>0</v>
+      </c>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
+      <c r="AP2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>0</v>
+      </c>
       <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="5"/>
+      <c r="AU2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA2" s="5">
+        <v>74.786324786324798</v>
+      </c>
+      <c r="BB2" s="6"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1">
+        <v>99</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>0</v>
+      </c>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
-      <c r="AP3" s="3"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="4"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="4"/>
-      <c r="AZ3" s="4"/>
-      <c r="BA3" s="5"/>
+      <c r="AP3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>101.248</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>40.367089999999997</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>11</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>0.14813999999999999</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>2.9974212906709865</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>74.786324786324798</v>
+      </c>
       <c r="BB3" s="6"/>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1">
+        <v>98</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>0</v>
+      </c>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="4"/>
+      <c r="AP4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>0</v>
+      </c>
       <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
-      <c r="BA4" s="5"/>
+      <c r="AU4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW4" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX4" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>74.786324786324798</v>
+      </c>
       <c r="BB4" s="6"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>0</v>
+      </c>
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="4"/>
+      <c r="AP5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="4">
+        <v>0</v>
+      </c>
       <c r="AT5" s="1"/>
-      <c r="AU5" s="1"/>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="4"/>
-      <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
-      <c r="BA5" s="5"/>
+      <c r="AU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>74.786324786324798</v>
+      </c>
       <c r="BB5" s="6"/>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1">
+        <v>87.4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>0</v>
+      </c>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
+      <c r="AP6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="4">
+        <v>0</v>
+      </c>
       <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
-      <c r="AY6" s="4"/>
-      <c r="AZ6" s="4"/>
-      <c r="BA6" s="5"/>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW6" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>74.786324786324798</v>
+      </c>
       <c r="BB6" s="6"/>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="1">
+        <v>84</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>16</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>0</v>
+      </c>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="4"/>
+      <c r="AP7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="4">
+        <v>0</v>
+      </c>
       <c r="AT7" s="1"/>
-      <c r="AU7" s="1"/>
-      <c r="AW7" s="4"/>
-      <c r="AX7" s="4"/>
-      <c r="AY7" s="4"/>
-      <c r="AZ7" s="4"/>
-      <c r="BA7" s="5"/>
+      <c r="AU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW7" s="4">
+        <v>350</v>
+      </c>
+      <c r="AX7" s="4">
+        <v>1200</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>130</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>30</v>
+      </c>
+      <c r="BA7" s="5">
+        <v>74.786324786324798</v>
+      </c>
       <c r="BB7" s="6"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -9250,7 +9913,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C8B63165-CF7D-4274-8182-15DC426AC4DA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Index calculations and analysis data prep and added a few examples in the template. Updated main.py to run the whole project.
</commit_message>
<xml_diff>
--- a/Alloy Template.xlsx
+++ b/Alloy Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bama365-my.sharepoint.com/personal/amjordan7_crimson_ua_edu/Documents/Documents/1 Projects/Research/3_AM-Hot Cracking ML-CALPHAD Project/3_hcm_calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="532" documentId="8_{21EBF174-53D2-406F-9F3E-90F98D5EF992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4627661-9CC2-44B9-9C89-6E733B5A3DB9}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{21EBF174-53D2-406F-9F3E-90F98D5EF992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DCF87D0-8C8C-426B-AE83-F1738F89857F}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="-9840" windowWidth="13350" windowHeight="21285" tabRatio="497" xr2:uid="{39467DA1-796B-4162-A05F-681B8E420767}"/>
+    <workbookView xWindow="28695" yWindow="-10620" windowWidth="16410" windowHeight="14505" tabRatio="497" xr2:uid="{39467DA1-796B-4162-A05F-681B8E420767}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -642,8 +642,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BB171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" activeCellId="6" sqref="AX1:AX1048576 AU1:AU1048576 AR1:AR1048576 AP1:AP1048576 E1:AM1048576 D1:D1048576 B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,10 @@
     <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="35" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.28515625" customWidth="1"/>
+    <col min="39" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.85546875" customWidth="1"/>
     <col min="44" max="44" width="9.7109375" customWidth="1"/>
     <col min="47" max="47" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="20.7109375" bestFit="1" customWidth="1"/>

</xml_diff>